<commit_message>
fix configur file bug
0.08g_1deg.xlsx
-0.15g_-1deg.xlsx
</commit_message>
<xml_diff>
--- a/2DPlatformControlSystem/Configure/丁玉玲/iTest配置文件/加速度配置文件/-0.08g_0.8s.xlsx
+++ b/2DPlatformControlSystem/Configure/丁玉玲/iTest配置文件/加速度配置文件/-0.08g_0.8s.xlsx
@@ -1,112 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="配置文件" sheetId="1" r:id="rId1"/>
+    <sheet name="配置文件" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">配置文件!$A$1:$B$3</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">配置文件!$A$1:$B$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>配置项目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>判断值</t>
   </si>
   <si>
     <t>运行模式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrdControl</t>
+  </si>
+  <si>
+    <t>表示肯定</t>
   </si>
   <si>
     <t>线性运动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>判断值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表示肯定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>表示否定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>延迟时间(s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线性运行设置为1，属性有效。</t>
   </si>
   <si>
     <t>加速时间(s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>减速时间(s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>最大速度(mm/s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>匀速时间(s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>转动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转动设置为1，属性有效。</t>
   </si>
   <si>
     <t>最大速度(deg/s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>转动角度(deg)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>数据采集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>扫描间隔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>采集频率=
 采集量/扫描间隔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集量</t>
   </si>
   <si>
     <t>取平均数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存文件类型是XLS时，属性有效</t>
   </si>
   <si>
     <t>是否作图1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>是否作图2</t>
@@ -119,169 +107,30 @@
   </si>
   <si>
     <t>表头名称1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH_1</t>
   </si>
   <si>
     <t>表头名称2</t>
   </si>
   <si>
+    <t>CH_2</t>
+  </si>
+  <si>
     <t>表头名称3</t>
   </si>
   <si>
+    <t>CH_3</t>
+  </si>
+  <si>
     <t>表头名称4</t>
   </si>
   <si>
-    <t>CH_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CH_2</t>
-  </si>
-  <si>
-    <t>CH_3</t>
+    <t>CH_4</t>
   </si>
   <si>
     <t>实验条件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保存文件类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保存文件名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不用加后缀名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>属性</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CH_4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XLS</t>
-  </si>
-  <si>
-    <t>TrdControl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-0.08g_0.8s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>线性运行</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>设置为1，属性有效。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>转动</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>设置为1，属性有效。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>保存文件类型是</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>XLS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>时，属性有效</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>填写</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>XLS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>或者</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>DAT</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Acc Time=0.8s Dec Time=0.4s
@@ -289,78 +138,96 @@
 Pre-Stop time=1s 
 Scan Intervals=200
 Date Size=1100000
-T=24.5 RH=15%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+T=17.5 RH=27.0%</t>
+  </si>
+  <si>
+    <t>保存文件类型</t>
+  </si>
+  <si>
+    <t>XLS</t>
+  </si>
+  <si>
+    <t>填写XLS或者DAT</t>
+  </si>
+  <si>
+    <t>保存文件名</t>
+  </si>
+  <si>
+    <t>-0.08g_0.8s</t>
+  </si>
+  <si>
+    <t>不用加后缀名</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <color rgb="FFFF0000"/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="7">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.3499862666707358"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,124 +294,67 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyProtection="1" borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyProtection="1" borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyProtection="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="1" fillId="5" fontId="2" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor theme="0" tint="-0.3499862666707358"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -810,19 +620,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="2"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="15.25"/>
+    <col customWidth="1" max="2" min="2" style="2" width="33.125"/>
+    <col customWidth="1" max="3" min="3" style="2" width="16.375"/>
+    <col customWidth="1" max="16384" min="4" style="2" width="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -830,359 +644,338 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="n"/>
+      <c r="G2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
       <c r="H2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="G3" s="5">
+      <c r="C3" s="7" t="n"/>
+      <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>0.8</v>
       </c>
-      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>0.4</v>
       </c>
-      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <v>-640</v>
       </c>
-      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="n">
         <v>0.05</v>
       </c>
-      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="5" t="n"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="9">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9" t="n">
         <v>0.1</v>
       </c>
-      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="n">
         <v>0.1</v>
       </c>
-      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="9">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9" t="n">
         <v>60</v>
       </c>
-      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="9">
+        <v>18</v>
+      </c>
+      <c r="B14" s="9" t="n">
         <v>60</v>
       </c>
-      <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="11">
+        <v>19</v>
+      </c>
+      <c r="B15" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="5" t="n"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="11">
+        <v>20</v>
+      </c>
+      <c r="B16" s="11" t="n">
         <v>200</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="11">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11" t="n">
         <v>1100000</v>
       </c>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="11">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11" t="n">
         <v>100</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="11">
+        <v>25</v>
+      </c>
+      <c r="B19" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="14"/>
-    </row>
-    <row r="20" spans="1:3">
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="11">
+        <v>26</v>
+      </c>
+      <c r="B20" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="14"/>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="11">
+        <v>27</v>
+      </c>
+      <c r="B21" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="1:3">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="11">
+        <v>28</v>
+      </c>
+      <c r="B22" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="1:3">
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="11" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="1:3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="11" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="14"/>
-    </row>
-    <row r="25" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="14"/>
-    </row>
-    <row r="26" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="11" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="14"/>
-    </row>
-    <row r="27" spans="1:3" ht="81">
+    </row>
+    <row customHeight="1" ht="81" r="27" spans="1:8">
       <c r="A27" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="14"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" autoFilter="0" pivotTables="0"/>
-  <dataConsolidate/>
   <mergeCells count="4">
     <mergeCell ref="C4:C8"/>
     <mergeCell ref="C10:C14"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C18:C27"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A3:B8">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule dxfId="0" priority="7" type="expression">
       <formula>$B$3=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B14">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule dxfId="0" priority="6" type="expression">
       <formula>$B$9=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:B27">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule dxfId="0" priority="8" type="expression">
       <formula>$B$28="DAT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B29">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule dxfId="0" priority="5" type="expression">
       <formula>$B$15=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule dxfId="0" priority="4" type="expression">
       <formula>$B$19=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule dxfId="0" priority="3" type="expression">
       <formula>$B$20=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule dxfId="0" priority="2" type="expression">
       <formula>$B$21=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule dxfId="0" priority="1" type="expression">
       <formula>$B$22=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:B21">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="B19:B21" type="list">
       <formula1>$G$2:$G$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="B28" type="list">
       <formula1>"DAT,XLS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="B22" type="list">
       <formula1>"1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B9 B15">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="B3 B9 B15" type="list">
       <formula1>"1,0"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>